<commit_message>
Master: airoldi e giani 17-05
</commit_message>
<xml_diff>
--- a/Lista schede alunno.xlsx
+++ b/Lista schede alunno.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elia Salerno\Desktop\ver_quinte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE8E58E-4322-477B-B86F-38C514B26E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2126878A-8871-4A28-A6B1-0A6936E59290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -701,7 +701,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -861,7 +861,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="4">
         <v>1.5</v>
@@ -879,7 +879,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -964,13 +964,15 @@
       <c r="G9" s="4">
         <v>2</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="4">
+        <v>3</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1279,12 +1281,10 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="4">
-        <v>1</v>
-      </c>
+      <c r="K21" s="4"/>
       <c r="L21" s="4">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>